<commit_message>
Mid target is completed
</commit_message>
<xml_diff>
--- a/Source Code/Regression Models Results/Results_Regression_Models.xlsx
+++ b/Source Code/Regression Models Results/Results_Regression_Models.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahmood Yousaf\Desktop\FYP\Final-Year-Project-Soil-Analysis-using-machine-learning\Source Code\Regression Models Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FB069C-68EA-4B92-9323-90026DD9EE2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73607AD7-B4F5-461B-B2BB-2EE29903086D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{53ECB87B-17D8-48DF-BAC0-311E968B74B5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="20">
   <si>
     <t>SVR</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>MAE</t>
-  </si>
-  <si>
-    <t>R2_Score</t>
   </si>
   <si>
     <t>ANN</t>
@@ -127,7 +124,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,6 +167,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -198,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -223,6 +226,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FFC2B9-50AD-40B7-A1D8-417082AF300E}">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="E36" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,148 +588,121 @@
     <row r="5" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="G5" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
+      <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="F6" s="1"/>
       <c r="G6" s="5"/>
       <c r="H6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="E7" s="1"/>
       <c r="G7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H7" s="6">
-        <v>-1.29E-2</v>
+        <v>0.65949999999999998</v>
       </c>
       <c r="I7" s="6">
         <v>1.7061999999999999</v>
-      </c>
-      <c r="J7" s="6">
-        <v>0.65949999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="E8" s="1"/>
       <c r="G8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H8" s="6">
-        <v>-0.56830000000000003</v>
+        <v>0.75849999999999995</v>
       </c>
       <c r="I8" s="6">
         <v>2.5181</v>
-      </c>
-      <c r="J8" s="6">
-        <v>0.75849999999999995</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="E9" s="1"/>
       <c r="G9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H9" s="6">
-        <v>-0.62960000000000005</v>
+        <v>1.1773</v>
       </c>
       <c r="I9" s="6">
         <v>2.3485</v>
-      </c>
-      <c r="J9" s="6">
-        <v>1.1773</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="E10" s="1"/>
       <c r="G10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H10" s="6">
-        <v>-58.4953</v>
+        <v>1.0085999999999999</v>
       </c>
       <c r="I10" s="6">
         <v>1.8620000000000001</v>
       </c>
-      <c r="J10" s="6">
-        <v>1.0085999999999999</v>
-      </c>
     </row>
     <row r="17" spans="7:16" ht="21" x14ac:dyDescent="0.35">
       <c r="G17" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
+      <c r="J17" s="12"/>
       <c r="M17" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N17" s="8"/>
       <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
+      <c r="P17" s="12"/>
     </row>
     <row r="18" spans="7:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G18" s="5"/>
       <c r="H18" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J18" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="M18" s="5"/>
       <c r="N18" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="P18" s="4" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="19" spans="7:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G19" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H19" s="6">
-        <v>-1.1900000000000001E-2</v>
+        <v>0.50390000000000001</v>
       </c>
       <c r="I19" s="6">
         <v>0.99950000000000006</v>
       </c>
-      <c r="J19" s="6">
-        <v>0.50390000000000001</v>
-      </c>
       <c r="M19" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N19" s="6">
-        <v>-1.01E-2</v>
+        <v>0.91710000000000003</v>
       </c>
       <c r="O19" s="6">
         <v>1.3756600000000001</v>
-      </c>
-      <c r="P19" s="6">
-        <v>0.91710000000000003</v>
       </c>
     </row>
     <row r="20" spans="7:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -730,25 +710,19 @@
         <v>1</v>
       </c>
       <c r="H20" s="6">
-        <v>-0.9143</v>
+        <v>0.53169999999999995</v>
       </c>
       <c r="I20" s="6">
         <v>1.0421</v>
       </c>
-      <c r="J20" s="6">
-        <v>0.53169999999999995</v>
-      </c>
       <c r="M20" s="4" t="s">
         <v>1</v>
       </c>
       <c r="N20" s="6">
-        <v>-0.55689999999999995</v>
+        <v>1.01294</v>
       </c>
       <c r="O20" s="6">
         <v>1.8266</v>
-      </c>
-      <c r="P20" s="6">
-        <v>1.01294</v>
       </c>
     </row>
     <row r="21" spans="7:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -756,25 +730,19 @@
         <v>2</v>
       </c>
       <c r="H21" s="6">
-        <v>-1.0121</v>
+        <v>0.51570000000000005</v>
       </c>
       <c r="I21" s="6">
         <v>1.7504</v>
       </c>
-      <c r="J21" s="6">
-        <v>0.51570000000000005</v>
-      </c>
       <c r="M21" s="4" t="s">
         <v>2</v>
       </c>
       <c r="N21" s="6">
-        <v>-0.505</v>
+        <v>1.0253000000000001</v>
       </c>
       <c r="O21" s="6">
         <v>2.1533000000000002</v>
-      </c>
-      <c r="P21" s="6">
-        <v>1.0253000000000001</v>
       </c>
     </row>
     <row r="22" spans="7:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -782,87 +750,69 @@
         <v>0</v>
       </c>
       <c r="H22" s="6">
-        <v>-4.7000000000000002E-3</v>
+        <v>0.53559999999999997</v>
       </c>
       <c r="I22" s="6">
         <v>1.9301999999999999</v>
       </c>
-      <c r="J22" s="6">
-        <v>0.53559999999999997</v>
-      </c>
       <c r="M22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="N22" s="6">
-        <v>-1.9539999999999998E-2</v>
+        <v>0.94840000000000002</v>
       </c>
       <c r="O22" s="6">
         <v>1.6386000000000001</v>
       </c>
-      <c r="P22" s="6">
-        <v>0.94840000000000002</v>
-      </c>
     </row>
     <row r="25" spans="7:16" ht="21" x14ac:dyDescent="0.35">
       <c r="G25" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
+      <c r="J25" s="12"/>
       <c r="M25" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
+      <c r="P25" s="12"/>
     </row>
     <row r="26" spans="7:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G26" s="5"/>
       <c r="H26" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J26" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="M26" s="5"/>
       <c r="N26" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O26" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="P26" s="4" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="27" spans="7:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G27" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H27" s="6">
-        <v>-6.7999999999999996E-3</v>
+        <v>0.16159999999999999</v>
       </c>
       <c r="I27" s="6">
         <v>3.9989999999999998E-2</v>
       </c>
-      <c r="J27" s="6">
-        <v>0.16159999999999999</v>
-      </c>
       <c r="M27" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N27" s="6">
-        <v>-6.1800000000000001E-2</v>
+        <v>0.1153</v>
       </c>
       <c r="O27" s="6">
         <v>2.1399999999999999E-2</v>
-      </c>
-      <c r="P27" s="6">
-        <v>0.1153</v>
       </c>
     </row>
     <row r="28" spans="7:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -870,25 +820,19 @@
         <v>1</v>
       </c>
       <c r="H28" s="6">
-        <v>-0.16800000000000001</v>
+        <v>0.15010999999999999</v>
       </c>
       <c r="I28" s="6">
         <v>3.6200000000000003E-2</v>
       </c>
-      <c r="J28" s="6">
-        <v>0.15010999999999999</v>
-      </c>
       <c r="M28" s="4" t="s">
         <v>1</v>
       </c>
       <c r="N28" s="6">
-        <v>-0.4022</v>
+        <v>0.1298</v>
       </c>
       <c r="O28" s="6">
         <v>3.32E-2</v>
-      </c>
-      <c r="P28" s="6">
-        <v>0.1298</v>
       </c>
     </row>
     <row r="29" spans="7:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -896,25 +840,19 @@
         <v>2</v>
       </c>
       <c r="H29" s="6">
-        <v>-0.4471</v>
+        <v>0.14419999999999999</v>
       </c>
       <c r="I29" s="6">
         <v>4.2840000000000003E-2</v>
       </c>
-      <c r="J29" s="6">
-        <v>0.14419999999999999</v>
-      </c>
       <c r="M29" s="4" t="s">
         <v>2</v>
       </c>
       <c r="N29" s="6">
-        <v>-0.7258</v>
+        <v>0.12759999999999999</v>
       </c>
       <c r="O29" s="6">
         <v>3.5700000000000003E-2</v>
-      </c>
-      <c r="P29" s="6">
-        <v>0.12759999999999999</v>
       </c>
     </row>
     <row r="30" spans="7:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -922,87 +860,69 @@
         <v>0</v>
       </c>
       <c r="H30" s="6">
-        <v>-1.7000000000000001E-2</v>
+        <v>0.14549999999999999</v>
       </c>
       <c r="I30" s="6">
         <v>3.2800000000000003E-2</v>
       </c>
-      <c r="J30" s="6">
-        <v>0.14549999999999999</v>
-      </c>
       <c r="M30" s="4" t="s">
         <v>0</v>
       </c>
       <c r="N30" s="6">
-        <v>-1.2200000000000001E-2</v>
+        <v>0.111</v>
       </c>
       <c r="O30" s="6">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="P30" s="6">
-        <v>0.111</v>
-      </c>
     </row>
     <row r="38" spans="7:16" ht="21" x14ac:dyDescent="0.35">
       <c r="G38" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
+      <c r="J38" s="12"/>
       <c r="M38" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N38" s="8"/>
       <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
+      <c r="P38" s="12"/>
     </row>
     <row r="39" spans="7:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G39" s="5"/>
       <c r="H39" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I39" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J39" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="M39" s="5"/>
       <c r="N39" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O39" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="P39" s="4" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="40" spans="7:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G40" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H40" s="6">
-        <v>-6.4000000000000003E-3</v>
+        <v>0.4677</v>
       </c>
       <c r="I40" s="6">
         <v>0.99400999999999995</v>
       </c>
-      <c r="J40" s="6">
-        <v>0.4677</v>
-      </c>
       <c r="M40" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N40" s="6">
-        <v>-0.34139999999999998</v>
+        <v>1.0794999999999999</v>
       </c>
       <c r="O40" s="6">
         <v>1.8267</v>
-      </c>
-      <c r="P40" s="6">
-        <v>1.0794999999999999</v>
       </c>
     </row>
     <row r="41" spans="7:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -1010,25 +930,19 @@
         <v>1</v>
       </c>
       <c r="H41" s="6">
-        <v>-0.2097</v>
+        <v>0.63529999999999998</v>
       </c>
       <c r="I41" s="6">
         <v>1.4531000000000001</v>
       </c>
-      <c r="J41" s="6">
-        <v>0.63529999999999998</v>
-      </c>
       <c r="M41" s="4" t="s">
         <v>1</v>
       </c>
       <c r="N41" s="6">
-        <v>-0.2162</v>
+        <v>0.97309999999999997</v>
       </c>
       <c r="O41" s="6">
         <v>1.6991000000000001</v>
-      </c>
-      <c r="P41" s="6">
-        <v>0.97309999999999997</v>
       </c>
     </row>
     <row r="42" spans="7:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -1036,25 +950,19 @@
         <v>2</v>
       </c>
       <c r="H42" s="6">
-        <v>-0.26469999999999999</v>
+        <v>0.70979999999999999</v>
       </c>
       <c r="I42" s="6">
         <v>1.7847999999999999</v>
       </c>
-      <c r="J42" s="6">
-        <v>0.70979999999999999</v>
-      </c>
       <c r="M42" s="4" t="s">
         <v>2</v>
       </c>
       <c r="N42" s="6">
-        <v>-0.3659</v>
+        <v>1.0696000000000001</v>
       </c>
       <c r="O42" s="6">
         <v>2.0878000000000001</v>
-      </c>
-      <c r="P42" s="6">
-        <v>1.0696000000000001</v>
       </c>
     </row>
     <row r="43" spans="7:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -1062,177 +970,141 @@
         <v>0</v>
       </c>
       <c r="H43" s="6">
-        <v>-1.06E-2</v>
+        <v>0.44919999999999999</v>
       </c>
       <c r="I43" s="6">
         <v>0.74639999999999995</v>
       </c>
-      <c r="J43" s="6">
-        <v>0.44919999999999999</v>
-      </c>
       <c r="M43" s="4" t="s">
         <v>0</v>
       </c>
       <c r="N43" s="6">
-        <v>1.44E-2</v>
+        <v>0.87860000000000005</v>
       </c>
       <c r="O43" s="6">
         <v>1.4257</v>
       </c>
-      <c r="P43" s="6">
-        <v>0.87860000000000005</v>
-      </c>
     </row>
     <row r="46" spans="7:16" ht="21" x14ac:dyDescent="0.35">
       <c r="G46" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H46" s="9"/>
       <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
+      <c r="J46" s="13"/>
       <c r="M46" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N46" s="10"/>
       <c r="O46" s="10"/>
-      <c r="P46" s="10"/>
+      <c r="P46" s="12"/>
     </row>
     <row r="47" spans="7:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G47" s="5"/>
       <c r="H47" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I47" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J47" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="M47" s="5"/>
       <c r="N47" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O47" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="P47" s="4" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="48" spans="7:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G48" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H48" s="6">
-        <v>-2.2252000000000001</v>
+        <v>0.29920000000000002</v>
       </c>
       <c r="I48" s="6">
         <v>0.12809999999999999</v>
       </c>
-      <c r="J48" s="6">
-        <v>0.29920000000000002</v>
-      </c>
       <c r="M48" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N48" s="6">
-        <v>-0.38779000000000002</v>
+        <v>0.1305</v>
       </c>
       <c r="O48" s="6">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="P48" s="6">
-        <v>0.1305</v>
-      </c>
-    </row>
-    <row r="49" spans="7:16" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="7:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G49" s="4" t="s">
         <v>1</v>
       </c>
       <c r="H49" s="6">
-        <v>-0.23619999999999999</v>
+        <v>0.15989999999999999</v>
       </c>
       <c r="I49" s="6">
         <v>4.1300000000000003E-2</v>
       </c>
-      <c r="J49" s="6">
-        <v>0.15989999999999999</v>
-      </c>
       <c r="M49" s="4" t="s">
         <v>1</v>
       </c>
       <c r="N49" s="6">
-        <v>-2.7400000000000001E-2</v>
+        <v>0.1532</v>
       </c>
       <c r="O49" s="6">
         <v>0.1368</v>
       </c>
-      <c r="P49" s="6">
-        <v>0.1532</v>
-      </c>
-    </row>
-    <row r="50" spans="7:16" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="7:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G50" s="4" t="s">
         <v>2</v>
       </c>
       <c r="H50" s="6">
-        <v>-0.1154</v>
+        <v>0.1552</v>
       </c>
       <c r="I50" s="6">
         <v>3.9699999999999999E-2</v>
       </c>
-      <c r="J50" s="6">
-        <v>0.1552</v>
-      </c>
       <c r="M50" s="4" t="s">
         <v>2</v>
       </c>
       <c r="N50" s="6">
-        <v>-0.33910000000000001</v>
+        <v>0.11990000000000001</v>
       </c>
       <c r="O50" s="6">
         <v>2.4E-2</v>
       </c>
-      <c r="P50" s="6">
-        <v>0.11990000000000001</v>
-      </c>
-    </row>
-    <row r="51" spans="7:16" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="7:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G51" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H51" s="6">
-        <v>-1.1900000000000001E-2</v>
+        <v>0.14319999999999999</v>
       </c>
       <c r="I51" s="6">
         <v>3.1800000000000002E-2</v>
       </c>
-      <c r="J51" s="6">
-        <v>0.14319999999999999</v>
-      </c>
       <c r="M51" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="N51" s="6">
-        <v>1.2999999999999999E-3</v>
-      </c>
+      <c r="N51" s="6"/>
       <c r="O51" s="6">
         <v>0.02</v>
       </c>
-      <c r="P51" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="G38:J38"/>
-    <mergeCell ref="M38:P38"/>
-    <mergeCell ref="G46:J46"/>
-    <mergeCell ref="M46:P46"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="M38:O38"/>
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="M46:O46"/>
     <mergeCell ref="E4:H4"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="M25:P25"/>
-    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="M25:O25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>